<commit_message>
add UI changes per pivot tab switch
</commit_message>
<xml_diff>
--- a/ExcelWebAddInFabricPivot/bin/Debug/Book1.xlsx
+++ b/ExcelWebAddInFabricPivot/bin/Debug/Book1.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R63d5fe3a04e74924"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R0e03478ac3594c5b"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R1b6a398ef15f49eb"/>
+  <wetp:taskpane dockstate="" visibility="1" width="700" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R087739043e1e4d00"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{df69ef57-a9e5-4e78-b5df-4767f1be2aa5}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{3638ad47-71e8-4432-8896-b1213e2adb45}">
   <we:reference id="a6de53a0-5db2-42bb-a5e0-9ed6c9a31f9d" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>